<commit_message>
added scrolling to line map; fixed number ordering problem in popups.
</commit_message>
<xml_diff>
--- a/data (in excel format)/genres.xlsx
+++ b/data (in excel format)/genres.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="176">
   <si>
     <t>poetid</t>
   </si>
@@ -518,9 +518,6 @@
     <t>Komos</t>
   </si>
   <si>
-    <t>(see Beazley ARV i 31)</t>
-  </si>
-  <si>
     <t>Prose</t>
   </si>
   <si>
@@ -552,15 +549,6 @@
   </si>
   <si>
     <t>Polemisterion</t>
-  </si>
-  <si>
-    <t>"Lyric"</t>
-  </si>
-  <si>
-    <t>"Melos"</t>
-  </si>
-  <si>
-    <t>Psogos</t>
   </si>
   <si>
     <t>Hyporchema</t>
@@ -1053,7 +1041,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1061,17 +1049,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F168"/>
+  <dimension ref="A1:F163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D162" sqref="D162:D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2229,41 +2218,41 @@
         <v>98</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>159</v>
+        <v>28</v>
       </c>
       <c r="D79">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F79" s="3"/>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B80">
-        <f>VLOOKUP(A80,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D80">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F80" s="3"/>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B81">
-        <v>99</v>
+        <f>VLOOKUP(A81,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>100</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>33</v>
+        <v>160</v>
       </c>
       <c r="D81">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F81" s="3"/>
     </row>
@@ -2276,10 +2265,10 @@
         <v>100</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>160</v>
+        <v>25</v>
       </c>
       <c r="D82">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F82" s="3"/>
     </row>
@@ -2292,10 +2281,10 @@
         <v>100</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D83">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F83" s="3"/>
     </row>
@@ -2308,10 +2297,10 @@
         <v>100</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D84">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F84" s="3"/>
     </row>
@@ -2324,10 +2313,10 @@
         <v>100</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D85">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F85" s="3"/>
     </row>
@@ -2340,10 +2329,10 @@
         <v>100</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>27</v>
+        <v>155</v>
       </c>
       <c r="D86">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F86" s="3"/>
     </row>
@@ -2356,10 +2345,10 @@
         <v>100</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="D87">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F87" s="3"/>
     </row>
@@ -2372,10 +2361,10 @@
         <v>100</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>179</v>
+        <v>34</v>
       </c>
       <c r="D88">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F88" s="3"/>
     </row>
@@ -2388,60 +2377,59 @@
         <v>100</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="D89">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F89" s="3"/>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B90">
         <f>VLOOKUP(A90,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="D90">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F90" s="3"/>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B91">
         <f>VLOOKUP(A91,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D91">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" s="3"/>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B92">
         <f>VLOOKUP(A92,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D92">
-        <v>2</v>
-      </c>
-      <c r="F92" s="3"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="1" t="s">
@@ -2452,34 +2440,34 @@
         <v>104</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D93">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B94">
         <f>VLOOKUP(A94,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D94">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B95">
         <f>VLOOKUP(A95,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>33</v>
@@ -2490,106 +2478,103 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B96">
         <f>VLOOKUP(A96,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="D96">
-        <v>23</v>
-      </c>
-      <c r="E96" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="1" t="s">
-        <v>116</v>
+        <v>39</v>
       </c>
       <c r="B97">
         <f>VLOOKUP(A97,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D97">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="1" t="s">
-        <v>116</v>
+        <v>39</v>
       </c>
       <c r="B98">
         <f>VLOOKUP(A98,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="D98">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="1" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
       <c r="B99">
         <f>VLOOKUP(A99,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D99">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="1" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="B100">
         <f>VLOOKUP(A100,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D100">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="1" t="s">
-        <v>117</v>
+        <v>152</v>
       </c>
       <c r="B101">
         <f>VLOOKUP(A101,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D101">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
-      <c r="A102" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B102">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" s="6" customFormat="1">
+      <c r="A102" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B102" s="6">
         <f>VLOOKUP(A102,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>111</v>
-      </c>
-      <c r="C102" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C102" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D102">
@@ -2598,32 +2583,32 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="1" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="B103">
         <f>VLOOKUP(A103,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>27</v>
+        <v>160</v>
       </c>
       <c r="D103">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" s="6" customFormat="1">
-      <c r="A104" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B104" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B104">
         <f>VLOOKUP(A104,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>113</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>33</v>
+        <v>114</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D104">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2635,10 +2620,10 @@
         <v>114</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D105">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2650,55 +2635,55 @@
         <v>114</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D106">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B107">
         <f>VLOOKUP(A107,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>162</v>
+        <v>99</v>
       </c>
       <c r="D107">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B108">
         <f>VLOOKUP(A108,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="D108">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B109">
         <f>VLOOKUP(A109,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
       <c r="D109">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2710,43 +2695,43 @@
         <v>116</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>99</v>
+        <v>170</v>
       </c>
       <c r="D110">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="E110" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B111">
         <f>VLOOKUP(A111,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>172</v>
+        <v>26</v>
       </c>
       <c r="D111">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B112">
         <f>VLOOKUP(A112,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>171</v>
+        <v>33</v>
       </c>
       <c r="D112">
-        <v>19</v>
-      </c>
-      <c r="E112" t="s">
-        <v>157</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2758,10 +2743,10 @@
         <v>118</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D113">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2773,10 +2758,10 @@
         <v>118</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D114">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2788,10 +2773,10 @@
         <v>118</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="D115">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2803,10 +2788,10 @@
         <v>118</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D116">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2818,49 +2803,49 @@
         <v>118</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="D117">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B118">
         <f>VLOOKUP(A118,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D118">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B119">
         <f>VLOOKUP(A119,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D119">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B120">
         <f>VLOOKUP(A120,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>25</v>
@@ -2871,131 +2856,131 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B121">
         <f>VLOOKUP(A121,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D121">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B122">
         <f>VLOOKUP(A122,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="D122">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B123">
         <f>VLOOKUP(A123,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D123">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B124">
         <f>VLOOKUP(A124,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="D124">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B125">
         <f>VLOOKUP(A125,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D125">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B126">
         <f>VLOOKUP(A126,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D126">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B127">
         <f>VLOOKUP(A127,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D127">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B128">
         <f>VLOOKUP(A128,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D128">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B129">
         <f>VLOOKUP(A129,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>33</v>
@@ -3006,11 +2991,11 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B130">
         <f>VLOOKUP(A130,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>28</v>
@@ -3021,137 +3006,137 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B131">
         <f>VLOOKUP(A131,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>159</v>
+        <v>33</v>
       </c>
       <c r="D131">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B132">
         <f>VLOOKUP(A132,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D132">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B133">
         <f>VLOOKUP(A133,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D133">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B134">
         <f>VLOOKUP(A134,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D134">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B135">
         <f>VLOOKUP(A135,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>99</v>
+        <v>33</v>
       </c>
       <c r="D135">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B136">
         <f>VLOOKUP(A136,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="D136">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B137">
         <f>VLOOKUP(A137,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>99</v>
+        <v>166</v>
       </c>
       <c r="D137">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B138">
         <f>VLOOKUP(A138,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D138">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B139">
         <f>VLOOKUP(A139,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="D139">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3163,10 +3148,10 @@
         <v>135</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>167</v>
+        <v>30</v>
       </c>
       <c r="D140">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -3178,10 +3163,10 @@
         <v>135</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D141">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -3193,139 +3178,139 @@
         <v>135</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>26</v>
+        <v>155</v>
       </c>
       <c r="D142">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B143">
         <f>VLOOKUP(A143,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D143">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B144">
         <f>VLOOKUP(A144,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="D144">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B145">
         <f>VLOOKUP(A145,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>160</v>
+        <v>33</v>
       </c>
       <c r="D145">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B146">
         <f>VLOOKUP(A146,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>155</v>
+        <v>31</v>
       </c>
       <c r="D146">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B147">
         <f>VLOOKUP(A147,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D147">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B148">
         <f>VLOOKUP(A148,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="D148">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B149">
         <f>VLOOKUP(A149,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D149">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150" s="1" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="B150">
         <f>VLOOKUP(A150,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>137</v>
+        <v>54</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>31</v>
+        <v>155</v>
       </c>
       <c r="D150">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B151">
         <f>VLOOKUP(A151,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>28</v>
@@ -3334,118 +3319,118 @@
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:4">
       <c r="A152" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B152">
         <f>VLOOKUP(A152,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="D152">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
       <c r="A153" s="1" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="B153">
         <f>VLOOKUP(A153,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="D153">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
       <c r="A154" s="1" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="B154">
         <f>VLOOKUP(A154,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>54</v>
+        <v>142</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="D154">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
       <c r="A155" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B155">
         <f>VLOOKUP(A155,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D155">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
       <c r="A156" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B156">
         <f>VLOOKUP(A156,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D156">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
       <c r="A157" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B157">
         <f>VLOOKUP(A157,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D157">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B158">
         <f>VLOOKUP(A158,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>179</v>
+        <v>31</v>
       </c>
       <c r="D158">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
       <c r="A159" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B159">
         <f>VLOOKUP(A159,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>33</v>
@@ -3454,145 +3439,66 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:4">
       <c r="A160" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B160">
         <f>VLOOKUP(A160,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>178</v>
+        <v>99</v>
       </c>
       <c r="D160">
-        <v>27</v>
-      </c>
-      <c r="E160" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
       <c r="A161" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B161">
         <f>VLOOKUP(A161,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>99</v>
+        <v>170</v>
       </c>
       <c r="D161">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
       <c r="A162" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B162">
         <f>VLOOKUP(A162,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D162">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5">
+        <f>VLOOKUP(C162,'genre lookup'!$A$1:$B$29,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
       <c r="A163" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B163">
         <f>VLOOKUP(A163,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>175</v>
+        <v>99</v>
       </c>
       <c r="D163">
-        <v>28</v>
-      </c>
-      <c r="E163" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5">
-      <c r="A164" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B164">
-        <f>VLOOKUP(A164,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>145</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D164">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5">
-      <c r="A165" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B165">
-        <f>VLOOKUP(A165,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>146</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D165">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5">
-      <c r="A166" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B166">
-        <f>VLOOKUP(A166,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>148</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D166">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B167">
-        <f>VLOOKUP(A167,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>148</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D167">
+        <f>VLOOKUP(C163,'genre lookup'!$A$1:$B$29,2,FALSE)</f>
         <v>11</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B168">
-        <f>VLOOKUP(A168,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
-        <v>148</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D168">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -4845,7 +4751,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B14">
         <v>14</v>
@@ -4869,7 +4775,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17">
         <v>17</v>
@@ -4877,7 +4783,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B18">
         <v>18</v>
@@ -4885,7 +4791,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B19">
         <v>19</v>
@@ -4909,7 +4815,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B22">
         <v>22</v>
@@ -4925,7 +4831,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B24">
         <v>24</v>
@@ -4933,7 +4839,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B25">
         <v>25</v>
@@ -4941,7 +4847,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B26">
         <v>26</v>
@@ -4949,7 +4855,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B27">
         <v>27</v>
@@ -4957,7 +4863,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B28">
         <v>28</v>
@@ -4965,7 +4871,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B29">
         <v>29</v>

</xml_diff>